<commit_message>
E2E dry run after creating all md files, and some fixes
</commit_message>
<xml_diff>
--- a/317 Newell St/Results/Excels/Performance_KPIs.xlsx
+++ b/317 Newell St/Results/Excels/Performance_KPIs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Total Investment</t>
+  </si>
+  <si>
+    <t>Cumulative Annual Cash Flow</t>
   </si>
   <si>
     <t>Home Value</t>
@@ -424,10 +427,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-7.913269501259248</v>
+        <v>-8.063701723164831</v>
       </c>
       <c r="C2">
-        <v>-3470.957834989838</v>
+        <v>-3536.941168323174</v>
       </c>
       <c r="D2">
         <v>43862.5</v>
@@ -438,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-2.044255865670737</v>
+        <v>-2.271415550291235</v>
       </c>
       <c r="C3">
-        <v>-896.6617290798272</v>
+        <v>-996.2996457464928</v>
       </c>
       <c r="D3">
         <v>43862.5</v>
@@ -452,10 +455,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-2.251724375217621</v>
+        <v>-2.481680939290951</v>
       </c>
       <c r="C4">
-        <v>-987.662604079829</v>
+        <v>-1088.527301996493</v>
       </c>
       <c r="D4">
         <v>43862.5</v>
@@ -466,10 +469,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-2.133461387186837</v>
+        <v>-2.369166865362006</v>
       </c>
       <c r="C5">
-        <v>-935.7895009548265</v>
+        <v>-1039.17581631941</v>
       </c>
       <c r="D5">
         <v>43862.5</v>
@@ -480,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-2.004771753209928</v>
+        <v>-2.246369868339475</v>
       </c>
       <c r="C6">
-        <v>-879.3430102517048</v>
+        <v>-985.3139835004019</v>
       </c>
       <c r="D6">
         <v>43862.5</v>
@@ -494,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-1.865424302948998</v>
+        <v>-2.113062370956774</v>
       </c>
       <c r="C7">
-        <v>-818.2217348810043</v>
+        <v>-926.841982460915</v>
       </c>
       <c r="D7">
         <v>43862.5</v>
@@ -508,10 +511,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-1.715183266640148</v>
+        <v>-1.969012286348124</v>
       </c>
       <c r="C8">
-        <v>-752.3222603300351</v>
+        <v>-863.6580140994458</v>
       </c>
       <c r="D8">
         <v>43862.5</v>
@@ -522,10 +525,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1.553808207301105</v>
+        <v>-1.813982952501783</v>
       </c>
       <c r="C9">
-        <v>-681.5391249274475</v>
+        <v>-795.6582725410947</v>
       </c>
       <c r="D9">
         <v>43862.5</v>
@@ -536,10 +539,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-1.381053953131822</v>
+        <v>-1.647733066962518</v>
       </c>
       <c r="C10">
-        <v>-605.7647901924454</v>
+        <v>-722.7369164964346</v>
       </c>
       <c r="D10">
         <v>43862.5</v>
@@ -550,10 +553,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.196670530188256</v>
+        <v>-1.470016621864718</v>
       </c>
       <c r="C11">
-        <v>-524.8896113038239</v>
+        <v>-644.7860407654121</v>
       </c>
       <c r="D11">
         <v>43862.5</v>
@@ -564,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-1.00040309541481</v>
+        <v>-1.280582839383189</v>
       </c>
       <c r="C12">
-        <v>-438.8018077263211</v>
+        <v>-561.6956479244512</v>
       </c>
       <c r="D12">
         <v>43862.5</v>
@@ -578,10 +581,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.7919918701261055</v>
+        <v>-1.079176107693683</v>
       </c>
       <c r="C13">
-        <v>-347.3874340340631</v>
+        <v>-473.3536202371417</v>
       </c>
       <c r="D13">
         <v>43862.5</v>
@@ -592,10 +595,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.5711720740339941</v>
+        <v>-0.8655359175407661</v>
       </c>
       <c r="C14">
-        <v>-250.5303509731606</v>
+        <v>-379.6456918313186</v>
       </c>
       <c r="D14">
         <v>43862.5</v>
@@ -606,10 +609,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.3376738599221271</v>
+        <v>-0.6393967995165766</v>
       </c>
       <c r="C15">
-        <v>-148.112196808343</v>
+        <v>-280.4554211879584</v>
       </c>
       <c r="D15">
         <v>43862.5</v>
@@ -620,10 +623,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.09122224907591338</v>
+        <v>-0.4004882621602184</v>
       </c>
       <c r="C16">
-        <v>-40.01235900092251</v>
+        <v>-175.6641639900258</v>
       </c>
       <c r="D16">
         <v>43862.5</v>
@@ -634,10 +637,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.1684629324176893</v>
+        <v>-0.1485347309937238</v>
       </c>
       <c r="C17">
-        <v>73.89205373170898</v>
+        <v>-65.1510463821221</v>
       </c>
       <c r="D17">
         <v>43862.5</v>
@@ -648,10 +651,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.4416671163793361</v>
+        <v>0.1167445113826356</v>
       </c>
       <c r="C18">
-        <v>193.7262389218863</v>
+        <v>51.20706130520853</v>
       </c>
       <c r="D18">
         <v>43862.5</v>
@@ -662,10 +665,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.7286810541273626</v>
+        <v>0.395635384005745</v>
       </c>
       <c r="C19">
-        <v>319.6177273666144</v>
+        <v>173.5355703095199</v>
       </c>
       <c r="D19">
         <v>43862.5</v>
@@ -676,10 +679,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.029800876813324</v>
+        <v>0.6884290649386676</v>
       </c>
       <c r="C20">
-        <v>451.696409592244</v>
+        <v>301.9621986087231</v>
       </c>
       <c r="D20">
         <v>43862.5</v>
@@ -690,10 +693,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1.345328154359864</v>
+        <v>0.9954220471883432</v>
       </c>
       <c r="C21">
-        <v>590.0945617060952</v>
+        <v>436.616995447987</v>
       </c>
       <c r="D21">
         <v>43862.5</v>
@@ -704,10 +707,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.675569952849638</v>
+        <v>1.31691619299882</v>
       </c>
       <c r="C22">
-        <v>734.9468705686722</v>
+        <v>577.6323651541073</v>
       </c>
       <c r="D22">
         <v>43862.5</v>
@@ -718,10 +721,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2.020838890205837</v>
+        <v>1.653218786358748</v>
       </c>
       <c r="C23">
-        <v>886.3904582165351</v>
+        <v>725.1430901666058</v>
       </c>
       <c r="D23">
         <v>43862.5</v>
@@ -732,10 +735,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2.381453189995681</v>
+        <v>2.00464258355242</v>
       </c>
       <c r="C24">
-        <v>1044.564905461856</v>
+        <v>879.2863532106803</v>
       </c>
       <c r="D24">
         <v>43862.5</v>
@@ -746,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2.757736733179434</v>
+        <v>2.371505861575081</v>
       </c>
       <c r="C25">
-        <v>1209.612274590829</v>
+        <v>1040.20175853337</v>
       </c>
       <c r="D25">
         <v>43862.5</v>
@@ -760,10 +763,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>3.150019107617313</v>
+        <v>2.754132464222861</v>
       </c>
       <c r="C26">
-        <v>1381.677131078644</v>
+        <v>1208.031352119752</v>
       </c>
       <c r="D26">
         <v>43862.5</v>
@@ -774,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.558635655137055</v>
+        <v>3.152851845657754</v>
       </c>
       <c r="C27">
-        <v>1560.90656423449</v>
+        <v>1382.919640801632</v>
       </c>
       <c r="D27">
         <v>43862.5</v>
@@ -788,10 +791,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>3.983927515953978</v>
+        <v>3.567999111237695</v>
       </c>
       <c r="C28">
-        <v>1747.450206685314</v>
+        <v>1565.013610166634</v>
       </c>
       <c r="D28">
         <v>43862.5</v>
@@ -802,10 +805,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4.426241670224277</v>
+        <v>3.999915055390085</v>
       </c>
       <c r="C29">
-        <v>1941.460252602124</v>
+        <v>1754.462741170476</v>
       </c>
       <c r="D29">
         <v>43862.5</v>
@@ -816,10 +819,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4.885930976501031</v>
+        <v>4.448946196295995</v>
       </c>
       <c r="C30">
-        <v>2143.091474567765</v>
+        <v>1951.419025350331</v>
       </c>
       <c r="D30">
         <v>43862.5</v>
@@ -830,10 +833,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>5.363354206849806</v>
+        <v>4.915444807139618</v>
       </c>
       <c r="C31">
-        <v>2352.501238979496</v>
+        <v>2156.036978531615</v>
       </c>
       <c r="D31">
         <v>43862.5</v>
@@ -844,10 +847,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.4377327180640288</v>
+        <v>0.4003309148295729</v>
       </c>
       <c r="C32">
-        <v>192.0005134608346</v>
+        <v>175.5951475171214</v>
       </c>
       <c r="D32">
         <v>43862.5</v>
@@ -860,21 +863,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -889,786 +892,879 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-3427.626729079823</v>
+        <v>-3502.86006241316</v>
       </c>
       <c r="C2">
+        <v>-3502.86006241316</v>
+      </c>
+      <c r="D2">
         <v>145000</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>37328.3525311382</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>11600</v>
       </c>
-      <c r="F2">
-        <v>22300.72580205838</v>
-      </c>
       <c r="G2">
+        <v>22225.49246872504</v>
+      </c>
+      <c r="H2">
         <v>-100</v>
       </c>
-      <c r="H2">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-1031.446729079827</v>
+        <v>-4632.911791492986</v>
       </c>
       <c r="C3">
+        <v>-1130.051729079826</v>
+      </c>
+      <c r="D3">
         <v>147900</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>41386.097073632</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>11832</v>
       </c>
-      <c r="F3">
-        <v>28522.65034455217</v>
-      </c>
       <c r="G3">
-        <v>-34.97258399646127</v>
+        <v>24921.18528213901</v>
       </c>
       <c r="H3">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-43.18339063633169</v>
+      </c>
+      <c r="I3">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-983.6822290798291</v>
+        <v>-5717.664145572812</v>
       </c>
       <c r="C4">
+        <v>-1084.752354079827</v>
+      </c>
+      <c r="D4">
         <v>150858</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>45587.07873961781</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>12068.64</v>
       </c>
-      <c r="F4">
-        <v>32534.75651053798</v>
-      </c>
       <c r="G4">
-        <v>-13.87542539640694</v>
+        <v>27800.774594045</v>
       </c>
       <c r="H4">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>-20.3874091192761</v>
+      </c>
+      <c r="I4">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-931.4356165798263</v>
+        <v>-6752.696640277639</v>
       </c>
       <c r="C5">
+        <v>-1035.032494704827</v>
+      </c>
+      <c r="D5">
         <v>153875.16</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>49938.732978432</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>12310.0128</v>
       </c>
-      <c r="F5">
-        <v>36697.28456185218</v>
-      </c>
       <c r="G5">
-        <v>-5.771954542934643</v>
+        <v>30876.02353815436</v>
       </c>
       <c r="H5">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>-11.04384681469495</v>
+      </c>
+      <c r="I5">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-874.6073187673301</v>
+        <v>-7733.490759123093</v>
       </c>
       <c r="C6">
+        <v>-980.7941188454542</v>
+      </c>
+      <c r="D6">
         <v>156952.6632</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>54448.98045951221</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>12556.213056</v>
       </c>
-      <c r="F6">
-        <v>41018.16008474488</v>
-      </c>
       <c r="G6">
-        <v>-1.662152328185096</v>
+        <v>34159.27664438912</v>
       </c>
       <c r="H6">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>-6.059293713488234</v>
+      </c>
+      <c r="I6">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-813.0957727095201</v>
+        <v>-8655.428001912685</v>
       </c>
       <c r="C7">
+        <v>-921.9372427895933</v>
+      </c>
+      <c r="D7">
         <v>160091.716464</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>59126.26155190052</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>12807.33731712</v>
       </c>
-      <c r="F7">
-        <v>45505.828462071</v>
-      </c>
       <c r="G7">
-        <v>0.738325780878224</v>
+        <v>37663.49623286783</v>
       </c>
       <c r="H7">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>-3.001403537028724</v>
+      </c>
+      <c r="I7">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-746.7973955682637</v>
+        <v>-9513.787904313027</v>
       </c>
       <c r="C8">
+        <v>-858.3599024003415</v>
+      </c>
+      <c r="D8">
         <v>163293.55079328</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>63979.57331736622</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>13063.4840634624</v>
       </c>
-      <c r="F8">
-        <v>50169.29185833555</v>
-      </c>
       <c r="G8">
-        <v>2.264311383763173</v>
+        <v>41402.30134959079</v>
       </c>
       <c r="H8">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>-0.9574416178019907</v>
+      </c>
+      <c r="I8">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-675.6065548691914</v>
+        <v>-10303.7460286851</v>
       </c>
       <c r="C9">
+        <v>-789.9581243720722</v>
+      </c>
+      <c r="D9">
         <v>166559.4218091457</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>69018.50920170991</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>13324.75374473165</v>
       </c>
-      <c r="F9">
-        <v>55018.14890210905</v>
-      </c>
       <c r="G9">
-        <v>3.290158029643386</v>
+        <v>45390.00942829315</v>
       </c>
       <c r="H9">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.4902303343547354</v>
+      </c>
+      <c r="I9">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-599.4155388581958</v>
+        <v>-11020.37192628375</v>
       </c>
       <c r="C10">
+        <v>-716.6258975986493</v>
+      </c>
+      <c r="D10">
         <v>169890.6102453286</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>74253.30162239051</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>13591.24881962629</v>
       </c>
-      <c r="F10">
-        <v>60062.63726390603</v>
-      </c>
       <c r="G10">
-        <v>4.007313094375431</v>
+        <v>49641.68087648048</v>
       </c>
       <c r="H10">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>1.559168650988907</v>
+      </c>
+      <c r="I10">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-518.1145269806992</v>
+        <v>-11658.62707097341</v>
       </c>
       <c r="C11">
+        <v>-638.2551446896632</v>
+      </c>
+      <c r="D11">
         <v>173288.4224502351</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>79694.86766519585</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>13863.07379601881</v>
       </c>
-      <c r="F11">
-        <v>65313.67934219634</v>
-      </c>
       <c r="G11">
-        <v>4.523106218223427</v>
+        <v>54173.16679820363</v>
       </c>
       <c r="H11">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>2.373575424871799</v>
+      </c>
+      <c r="I11">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-431.5915605213776</v>
+        <v>-12213.36276464648</v>
       </c>
       <c r="C12">
+        <v>-554.7356936730683</v>
+      </c>
+      <c r="D12">
         <v>176754.1908992399</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>85354.8581183261</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>14140.33527193919</v>
       </c>
-      <c r="F12">
-        <v>70782.93128586553</v>
-      </c>
       <c r="G12">
-        <v>4.901939126421939</v>
+        <v>59001.16008174044</v>
       </c>
       <c r="H12">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>3.009366656605827</v>
+      </c>
+      <c r="I12">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-339.7325134443072</v>
+        <v>-12679.31801457126</v>
       </c>
       <c r="C13">
+        <v>-465.9552499247848</v>
+      </c>
+      <c r="D13">
         <v>180289.2747172246</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>91245.71008906394</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>14423.14197737797</v>
       </c>
-      <c r="F13">
-        <v>76482.83559824165</v>
-      </c>
       <c r="G13">
-        <v>5.184530482999983</v>
+        <v>64143.2500971147</v>
       </c>
       <c r="H13">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>3.515464338428131</v>
+      </c>
+      <c r="I13">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-242.4210634757837</v>
+        <v>-13051.11738293954</v>
       </c>
       <c r="C14">
+        <v>-371.7993683682762</v>
+      </c>
+      <c r="D14">
         <v>183895.0602115691</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>97380.70346624395</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>14711.60481692553</v>
       </c>
-      <c r="F14">
-        <v>82426.67758584264</v>
-      </c>
       <c r="G14">
-        <v>5.397716351817183</v>
+        <v>69617.98126637889</v>
       </c>
       <c r="H14">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>3.924753652879165</v>
+      </c>
+      <c r="I14">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-139.5386634749393</v>
+        <v>-13323.26880892929</v>
       </c>
       <c r="C15">
+        <v>-272.1514259897477</v>
+      </c>
+      <c r="D15">
         <v>187572.9614158005</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>103774.0215111019</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>15005.83691326404</v>
       </c>
-      <c r="F15">
-        <v>88628.64593436294</v>
-      </c>
       <c r="G15">
-        <v>5.559790086662342</v>
+        <v>75444.91578890859</v>
       </c>
       <c r="H15">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>4.260115033245682</v>
+      </c>
+      <c r="I15">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-30.96451313964826</v>
+        <v>-13490.16140364661</v>
       </c>
       <c r="C16">
+        <v>-166.8925947173238</v>
+      </c>
+      <c r="D16">
         <v>191324.4206441165</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>110440.8158798777</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>15305.95365152932</v>
       </c>
-      <c r="F16">
-        <v>95103.89771520876</v>
-      </c>
       <c r="G16">
-        <v>5.683574868209718</v>
+        <v>81644.70082470181</v>
       </c>
       <c r="H16">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>4.537931271998419</v>
+      </c>
+      <c r="I16">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>83.42446890183237</v>
+        <v>-13546.0632183619</v>
       </c>
       <c r="C17">
+        <v>-55.90181471528558</v>
+      </c>
+      <c r="D17">
         <v>195150.9090569989</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>117397.2764038702</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>15612.07272455991</v>
       </c>
-      <c r="F17">
-        <v>101868.6281482122</v>
-      </c>
       <c r="G17">
-        <v>5.778272895839698</v>
+        <v>88239.14046094843</v>
       </c>
       <c r="H17">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>4.770220802404679</v>
+      </c>
+      <c r="I17">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>203.753672560073</v>
+        <v>-13485.11898650937</v>
       </c>
       <c r="C18">
+        <v>60.94423185252617</v>
+      </c>
+      <c r="D18">
         <v>199053.9272381389</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>124660.7059766082</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>15924.31417905111</v>
       </c>
-      <c r="F18">
-        <v>108940.1454701172</v>
-      </c>
       <c r="G18">
-        <v>5.850621082545659</v>
+        <v>95251.27281104775</v>
       </c>
       <c r="H18">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>4.965985570625864</v>
+      </c>
+      <c r="I18">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>330.1508232581182</v>
+        <v>-13301.34783997649</v>
       </c>
       <c r="C19">
+        <v>183.771146532883</v>
+      </c>
+      <c r="D19">
         <v>203035.0057829016</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>132249.6009235359</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>16242.80046263213</v>
       </c>
-      <c r="F19">
-        <v>116336.9512841619</v>
-      </c>
       <c r="G19">
-        <v>5.905636892291777</v>
+        <v>102705.4526209273</v>
       </c>
       <c r="H19">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>5.132090723338067</v>
+      </c>
+      <c r="I19">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>462.7460083498918</v>
+        <v>-12988.64100026996</v>
       </c>
       <c r="C20">
+        <v>312.7068397065268</v>
+      </c>
+      <c r="D20">
         <v>207095.7058985597</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>140183.7372572338</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>16567.65647188477</v>
       </c>
-      <c r="F20">
-        <v>124078.826793699</v>
-      </c>
       <c r="G20">
-        <v>5.947113170244278</v>
+        <v>110627.4397850791</v>
       </c>
       <c r="H20">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>5.273855033289565</v>
+      </c>
+      <c r="I20">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>601.6717029202955</v>
+        <v>-12540.75944520912</v>
       </c>
       <c r="C21">
+        <v>447.881555060847</v>
+      </c>
+      <c r="D21">
         <v>211237.6200165309</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>148484.2632508595</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>16899.00960132247</v>
       </c>
-      <c r="F21">
-        <v>132186.9253524573</v>
-      </c>
       <c r="G21">
-        <v>5.977954442043409</v>
+        <v>119044.4942043279</v>
       </c>
       <c r="H21">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>5.395456974760782</v>
+      </c>
+      <c r="I21">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>747.0627949003429</v>
+        <v>-11951.33155186471</v>
       </c>
       <c r="C22">
+        <v>589.4278933444037</v>
+      </c>
+      <c r="D22">
         <v>215462.3724168615</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>157173.7987943304</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>17236.98979334892</v>
       </c>
-      <c r="F22">
-        <v>140683.8717958818</v>
-      </c>
       <c r="G22">
-        <v>6.000410357771546</v>
+        <v>127985.4774491168</v>
       </c>
       <c r="H22">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>5.500220076310836</v>
+      </c>
+      <c r="I22">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>899.056609427098</v>
+        <v>-11213.85071653245</v>
       </c>
       <c r="C23">
+        <v>737.4808353322605</v>
+      </c>
+      <c r="D23">
         <v>219771.6198651987</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>166276.5420319646</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>17581.7295892159</v>
       </c>
-      <c r="F23">
-        <v>149593.8690521758</v>
-      </c>
       <c r="G23">
-        <v>6.016240801999073</v>
+        <v>137480.9617262163</v>
       </c>
       <c r="H23">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>5.590817299935957</v>
+      </c>
+      <c r="I23">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1057.792932374106</v>
+        <v>-10321.67295260555</v>
       </c>
       <c r="C24">
+        <v>892.1777639269003</v>
+      </c>
+      <c r="D24">
         <v>224167.0522625027</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>175818.3838169923</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>17933.36418100022</v>
       </c>
-      <c r="F24">
-        <v>158942.8125683662</v>
-      </c>
       <c r="G24">
-        <v>6.026834638914225</v>
+        <v>147563.3466833866</v>
       </c>
       <c r="H24">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>5.669419938079145</v>
+      </c>
+      <c r="I24">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1223.414032974168</v>
+        <v>-9268.014467289775</v>
       </c>
       <c r="C25">
+        <v>1053.658485315776</v>
+      </c>
+      <c r="D25">
         <v>228650.3933077528</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>185827.0305577619</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>18292.03146462022</v>
       </c>
-      <c r="F25">
-        <v>168758.4131261158</v>
-      </c>
       <c r="G25">
-        <v>6.033296400952826</v>
+        <v>158266.9846258519</v>
       </c>
       <c r="H25">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>5.737807762765801</v>
+      </c>
+      <c r="I25">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1396.064685451779</v>
+        <v>-8045.949218187843</v>
       </c>
       <c r="C26">
+        <v>1222.065249101932</v>
+      </c>
+      <c r="D26">
         <v>233223.4011739078</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>196332.1360727677</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>18657.87209391263</v>
       </c>
-      <c r="F26">
-        <v>179070.3286643068</v>
-      </c>
       <c r="G26">
-        <v>6.036510435429321</v>
+        <v>169628.3147606672</v>
       </c>
       <c r="H26">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>5.79745164498966</v>
+      </c>
+      <c r="I26">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1575.892189578373</v>
+        <v>-6648.406450868057</v>
       </c>
       <c r="C27">
+        <v>1397.542767319787</v>
+      </c>
+      <c r="D27">
         <v>237887.869197386</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>207365.4431170509</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>19031.02953579088</v>
       </c>
-      <c r="F27">
-        <v>189910.3057708385</v>
-      </c>
       <c r="G27">
-        <v>6.03718895537404</v>
+        <v>181686.007130392</v>
       </c>
       <c r="H27">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>5.849576308142423</v>
+      </c>
+      <c r="I27">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1763.046390058672</v>
+        <v>-5068.168218624437</v>
       </c>
       <c r="C28">
+        <v>1580.23823224362</v>
+      </c>
+      <c r="D28">
         <v>242645.6265813337</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>218960.9352912861</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>19411.6501265067</v>
       </c>
-      <c r="F28">
-        <v>201312.3315548381</v>
-      </c>
       <c r="G28">
-        <v>6.035908436611637</v>
+        <v>194481.116946155</v>
       </c>
       <c r="H28">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>5.895208541623909</v>
+      </c>
+      <c r="I28">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1957.679694651528</v>
+        <v>-3297.866885733338</v>
       </c>
       <c r="C29">
+        <v>1770.301332891099</v>
+      </c>
+      <c r="D29">
         <v>247498.5391129604</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>231155.0000972244</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>19799.88312903683</v>
       </c>
-      <c r="F29">
-        <v>213312.7966628391</v>
-      </c>
       <c r="G29">
-        <v>6.03313746964127</v>
+        <v>208057.2500824542</v>
       </c>
       <c r="H29">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>5.935214634417973</v>
+      </c>
+      <c r="I29">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2159.947090923786</v>
+        <v>-1329.982615613986</v>
       </c>
       <c r="C30">
+        <v>1967.884270119352</v>
+      </c>
+      <c r="D30">
         <v>252448.5098952196</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>243986.6039593715</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>20195.88079161757</v>
       </c>
-      <c r="F30">
-        <v>225950.6702586778</v>
-      </c>
       <c r="G30">
-        <v>6.029258272595839</v>
+        <v>222460.74055214</v>
       </c>
       <c r="H30">
-        <v>43862.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>5.970329720905032</v>
+      </c>
+      <c r="I30">
+        <v>43862.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2370.006161530016</v>
+        <v>843.1591545914707</v>
       </c>
       <c r="C31">
+        <v>2173.141770205457</v>
+      </c>
+      <c r="D31">
         <v>257497.480093124</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>257497.480093127</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>20599.79840744992</v>
       </c>
-      <c r="F31">
-        <v>239267.6878472071</v>
-      </c>
       <c r="G31">
-        <v>6.024583451562426</v>
+        <v>237740.8408402685</v>
       </c>
       <c r="H31">
+        <v>6.001180992228905</v>
+      </c>
+      <c r="I31">
         <v>43862.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added documentation compiling into 1 pdf
</commit_message>
<xml_diff>
--- a/317 Newell St/Results/Excels/Performance_KPIs.xlsx
+++ b/317 Newell St/Results/Excels/Performance_KPIs.xlsx
@@ -427,10 +427,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-8.063701723164831</v>
+        <v>-7.852283465351582</v>
       </c>
       <c r="C2">
-        <v>-3536.941168323174</v>
+        <v>-3444.207834989838</v>
       </c>
       <c r="D2">
         <v>43862.5</v>
@@ -441,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-2.271415550291235</v>
+        <v>-1.952164101635395</v>
       </c>
       <c r="C3">
-        <v>-996.2996457464928</v>
+        <v>-856.2679790798252</v>
       </c>
       <c r="D3">
         <v>43862.5</v>
@@ -455,10 +455,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-2.481680939290951</v>
+        <v>-2.158498741133831</v>
       </c>
       <c r="C4">
-        <v>-1088.527301996493</v>
+        <v>-946.7715103298265</v>
       </c>
       <c r="D4">
         <v>43862.5</v>
@@ -469,10 +469,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-2.369166865362006</v>
+        <v>-2.037905112250963</v>
       </c>
       <c r="C5">
-        <v>-1039.17581631941</v>
+        <v>-893.8761298610789</v>
       </c>
       <c r="D5">
         <v>43862.5</v>
@@ -483,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-2.246369868339475</v>
+        <v>-1.906826571400646</v>
       </c>
       <c r="C6">
-        <v>-985.3139835004019</v>
+        <v>-836.3818048806086</v>
       </c>
       <c r="D6">
         <v>43862.5</v>
@@ -497,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-2.113062370956774</v>
+        <v>-1.765030491594487</v>
       </c>
       <c r="C7">
-        <v>-926.841982460915</v>
+        <v>-774.1864993756319</v>
       </c>
       <c r="D7">
         <v>43862.5</v>
@@ -511,10 +511,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-1.969012286348124</v>
+        <v>-1.612279610001771</v>
       </c>
       <c r="C8">
-        <v>-863.6580140994458</v>
+        <v>-707.1861439370266</v>
       </c>
       <c r="D8">
         <v>43862.5</v>
@@ -525,10 +525,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1.813982952501783</v>
+        <v>-1.448331959246771</v>
       </c>
       <c r="C9">
-        <v>-795.6582725410947</v>
+        <v>-635.2746056246151</v>
       </c>
       <c r="D9">
         <v>43862.5</v>
@@ -539,10 +539,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-1.647733066962518</v>
+        <v>-1.272940798876131</v>
       </c>
       <c r="C10">
-        <v>-722.7369164964346</v>
+        <v>-558.3436579070431</v>
       </c>
       <c r="D10">
         <v>43862.5</v>
@@ -553,10 +553,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.470016621864718</v>
+        <v>-1.085854547076172</v>
       </c>
       <c r="C11">
-        <v>-644.7860407654121</v>
+        <v>-476.2829507112858</v>
       </c>
       <c r="D11">
         <v>43862.5</v>
@@ -567,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-1.280582839383189</v>
+        <v>-0.8868167127249336</v>
       </c>
       <c r="C12">
-        <v>-561.6956479244512</v>
+        <v>-388.979980618974</v>
       </c>
       <c r="D12">
         <v>43862.5</v>
@@ -581,10 +581,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-1.079176107693683</v>
+        <v>-0.675565827868966</v>
       </c>
       <c r="C13">
-        <v>-473.3536202371417</v>
+        <v>-296.3200612490252</v>
       </c>
       <c r="D13">
         <v>43862.5</v>
@@ -595,10 +595,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.8655359175407661</v>
+        <v>-0.4518353807204318</v>
       </c>
       <c r="C14">
-        <v>-379.6456918313186</v>
+        <v>-198.1862938684994</v>
       </c>
       <c r="D14">
         <v>43862.5</v>
@@ -609,10 +609,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.6393967995165766</v>
+        <v>-0.2153537492757411</v>
       </c>
       <c r="C15">
-        <v>-280.4554211879584</v>
+        <v>-94.45953827607195</v>
       </c>
       <c r="D15">
         <v>43862.5</v>
@@ -623,10 +623,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.4004882621602184</v>
+        <v>0.03415586433664432</v>
       </c>
       <c r="C16">
-        <v>-175.6641639900258</v>
+        <v>14.98161599466062</v>
       </c>
       <c r="D16">
         <v>43862.5</v>
@@ -637,10 +637,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-0.1485347309937238</v>
+        <v>0.2969754986655694</v>
       </c>
       <c r="C17">
-        <v>-65.1510463821221</v>
+        <v>130.2608781021854</v>
       </c>
       <c r="D17">
         <v>43862.5</v>
@@ -651,10 +651,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.1167445113826356</v>
+        <v>0.5733924967834013</v>
       </c>
       <c r="C18">
-        <v>51.20706130520853</v>
+        <v>251.5042839016194</v>
       </c>
       <c r="D18">
         <v>43862.5</v>
@@ -665,10 +665,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.395635384005745</v>
+        <v>0.8636995690415287</v>
       </c>
       <c r="C19">
-        <v>173.5355703095199</v>
+        <v>378.8402234708405</v>
       </c>
       <c r="D19">
         <v>43862.5</v>
@@ -679,10 +679,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.6884290649386676</v>
+        <v>1.168194854600343</v>
       </c>
       <c r="C20">
-        <v>301.9621986087231</v>
+        <v>512.3994680990755</v>
       </c>
       <c r="D20">
         <v>43862.5</v>
@@ -693,10 +693,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0.9954220471883432</v>
+        <v>1.487181981591563</v>
       </c>
       <c r="C21">
-        <v>436.616995447987</v>
+        <v>652.3151966755995</v>
       </c>
       <c r="D21">
         <v>43862.5</v>
@@ -707,10 +707,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.31691619299882</v>
+        <v>1.820970125762113</v>
       </c>
       <c r="C22">
-        <v>577.6323651541073</v>
+        <v>798.723021412407</v>
       </c>
       <c r="D22">
         <v>43862.5</v>
@@ -721,10 +721,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1.653218786358748</v>
+        <v>2.169874067441133</v>
       </c>
       <c r="C23">
-        <v>725.1430901666058</v>
+        <v>951.7610128313668</v>
       </c>
       <c r="D23">
         <v>43862.5</v>
@@ -735,10 +735,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2.00464258355242</v>
+        <v>2.534214246661863</v>
       </c>
       <c r="C24">
-        <v>879.2863532106803</v>
+        <v>1111.56972394206</v>
       </c>
       <c r="D24">
         <v>43862.5</v>
@@ -749,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2.371505861575081</v>
+        <v>2.91431681626227</v>
       </c>
       <c r="C25">
-        <v>1040.20175853337</v>
+        <v>1278.292213533038</v>
       </c>
       <c r="D25">
         <v>43862.5</v>
@@ -763,10 +763,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2.754132464222861</v>
+        <v>3.310513692777216</v>
       </c>
       <c r="C26">
-        <v>1208.031352119752</v>
+        <v>1452.074068494407</v>
       </c>
       <c r="D26">
         <v>43862.5</v>
@@ -777,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.152851845657754</v>
+        <v>3.72314260492597</v>
       </c>
       <c r="C27">
-        <v>1382.919640801632</v>
+        <v>1633.063425085654</v>
       </c>
       <c r="D27">
         <v>43862.5</v>
@@ -791,10 +791,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>3.567999111237695</v>
+        <v>4.152547139487621</v>
       </c>
       <c r="C28">
-        <v>1565.013610166634</v>
+        <v>1821.410989057758</v>
       </c>
       <c r="D28">
         <v>43862.5</v>
@@ -805,10 +805,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>3.999915055390085</v>
+        <v>4.599076784346256</v>
       </c>
       <c r="C29">
-        <v>1754.462741170476</v>
+        <v>2017.270054533877</v>
       </c>
       <c r="D29">
         <v>43862.5</v>
@@ -819,10 +819,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4.448946196295995</v>
+        <v>5.063086968476059</v>
       </c>
       <c r="C30">
-        <v>1951.419025350331</v>
+        <v>2220.796521547811</v>
       </c>
       <c r="D30">
         <v>43862.5</v>
@@ -833,10 +833,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>4.915444807139618</v>
+        <v>5.544939098624205</v>
       </c>
       <c r="C31">
-        <v>2156.036978531615</v>
+        <v>2432.148912134042</v>
       </c>
       <c r="D31">
         <v>43862.5</v>
@@ -847,10 +847,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.4003309148295729</v>
+        <v>0.4528956112671862</v>
       </c>
       <c r="C32">
-        <v>175.5951475171214</v>
+        <v>198.6513374920696</v>
       </c>
       <c r="D32">
         <v>43862.5</v>
@@ -903,10 +903,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-3502.86006241316</v>
+        <v>-3397.126729079823</v>
       </c>
       <c r="C2">
-        <v>-3502.86006241316</v>
+        <v>-3397.126729079823</v>
       </c>
       <c r="D2">
         <v>145000</v>
@@ -918,7 +918,7 @@
         <v>11600</v>
       </c>
       <c r="G2">
-        <v>22225.49246872504</v>
+        <v>22331.22580205838</v>
       </c>
       <c r="H2">
         <v>-100</v>
@@ -932,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-4632.911791492986</v>
+        <v>-4388.598458159649</v>
       </c>
       <c r="C3">
-        <v>-1130.051729079826</v>
+        <v>-991.4717290798253</v>
       </c>
       <c r="D3">
         <v>147900</v>
@@ -947,10 +947,10 @@
         <v>11832</v>
       </c>
       <c r="G3">
-        <v>24921.18528213901</v>
+        <v>25165.49861547235</v>
       </c>
       <c r="H3">
-        <v>-43.18339063633169</v>
+        <v>-42.62639244121436</v>
       </c>
       <c r="I3">
         <v>43862.5</v>
@@ -961,10 +961,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-5717.664145572812</v>
+        <v>-5331.306312239475</v>
       </c>
       <c r="C4">
-        <v>-1084.752354079827</v>
+        <v>-942.7078540798266</v>
       </c>
       <c r="D4">
         <v>150858</v>
@@ -976,10 +976,10 @@
         <v>12068.64</v>
       </c>
       <c r="G4">
-        <v>27800.774594045</v>
+        <v>28187.13242737833</v>
       </c>
       <c r="H4">
-        <v>-20.3874091192761</v>
+        <v>-19.83611481913701</v>
       </c>
       <c r="I4">
         <v>43862.5</v>
@@ -990,10 +990,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-6752.696640277639</v>
+        <v>-6220.743194444304</v>
       </c>
       <c r="C5">
-        <v>-1035.032494704827</v>
+        <v>-889.4368822048291</v>
       </c>
       <c r="D5">
         <v>153875.16</v>
@@ -1005,10 +1005,10 @@
         <v>12310.0128</v>
       </c>
       <c r="G5">
-        <v>30876.02353815436</v>
+        <v>31407.9769839877</v>
       </c>
       <c r="H5">
-        <v>-11.04384681469495</v>
+        <v>-10.5358868994265</v>
       </c>
       <c r="I5">
         <v>43862.5</v>
@@ -1019,10 +1019,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-7733.490759123093</v>
+        <v>-7052.301810477256</v>
       </c>
       <c r="C6">
-        <v>-980.7941188454542</v>
+        <v>-831.5586160329522</v>
       </c>
       <c r="D6">
         <v>156952.6632</v>
@@ -1034,10 +1034,10 @@
         <v>12556.213056</v>
       </c>
       <c r="G6">
-        <v>34159.27664438912</v>
+        <v>34840.46559303495</v>
       </c>
       <c r="H6">
-        <v>-6.059293713488234</v>
+        <v>-5.594424899848416</v>
       </c>
       <c r="I6">
         <v>43862.5</v>
@@ -1048,10 +1048,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-8655.428001912685</v>
+        <v>-7821.272662884041</v>
       </c>
       <c r="C7">
-        <v>-921.9372427895933</v>
+        <v>-768.9708524067846</v>
       </c>
       <c r="D7">
         <v>160091.716464</v>
@@ -1063,10 +1063,10 @@
         <v>12807.33731712</v>
       </c>
       <c r="G7">
-        <v>37663.49623286783</v>
+        <v>38497.65157189648</v>
       </c>
       <c r="H7">
-        <v>-3.001403537028724</v>
+        <v>-2.57550321425799</v>
       </c>
       <c r="I7">
         <v>43862.5</v>
@@ -1077,10 +1077,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-9513.787904313027</v>
+        <v>-8522.842015142</v>
       </c>
       <c r="C8">
-        <v>-858.3599024003415</v>
+        <v>-701.5693522579577</v>
       </c>
       <c r="D8">
         <v>163293.55079328</v>
@@ -1092,10 +1092,10 @@
         <v>13063.4840634624</v>
       </c>
       <c r="G8">
-        <v>41402.30134959079</v>
+        <v>42393.24723876181</v>
       </c>
       <c r="H8">
-        <v>-0.9574416178019907</v>
+        <v>-0.5662350551105422</v>
       </c>
       <c r="I8">
         <v>43862.5</v>
@@ -1106,10 +1106,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-10303.7460286851</v>
+        <v>-9152.089825618128</v>
       </c>
       <c r="C9">
-        <v>-789.9581243720722</v>
+        <v>-629.2478104761294</v>
       </c>
       <c r="D9">
         <v>166559.4218091457</v>
@@ -1121,10 +1121,10 @@
         <v>13324.75374473165</v>
       </c>
       <c r="G9">
-        <v>45390.00942829315</v>
+        <v>46541.66563136013</v>
       </c>
       <c r="H9">
-        <v>0.4902303343547354</v>
+        <v>0.8505713411053994</v>
       </c>
       <c r="I9">
         <v>43862.5</v>
@@ -1135,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-11020.37192628375</v>
+        <v>-9703.987651473435</v>
       </c>
       <c r="C10">
-        <v>-716.6258975986493</v>
+        <v>-551.8978258553079</v>
       </c>
       <c r="D10">
         <v>169890.6102453286</v>
@@ -1150,10 +1150,10 @@
         <v>13591.24881962629</v>
       </c>
       <c r="G10">
-        <v>49641.68087648048</v>
+        <v>50958.06515129079</v>
       </c>
       <c r="H10">
-        <v>1.559168650988907</v>
+        <v>1.891966364283193</v>
       </c>
       <c r="I10">
         <v>43862.5</v>
@@ -1164,10 +1164,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-11658.62707097341</v>
+        <v>-10173.39652262617</v>
       </c>
       <c r="C11">
-        <v>-638.2551446896632</v>
+        <v>-469.4088711527384</v>
       </c>
       <c r="D11">
         <v>173288.4224502351</v>
@@ -1179,10 +1179,10 @@
         <v>13863.07379601881</v>
       </c>
       <c r="G11">
-        <v>54173.16679820363</v>
+        <v>55658.39734655086</v>
       </c>
       <c r="H11">
-        <v>2.373575424871799</v>
+        <v>2.681696413227197</v>
       </c>
       <c r="I11">
         <v>43862.5</v>
@@ -1193,10 +1193,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-12213.36276464648</v>
+        <v>-10555.0647859239</v>
       </c>
       <c r="C12">
-        <v>-554.7356936730683</v>
+        <v>-381.6682632977227</v>
       </c>
       <c r="D12">
         <v>176754.1908992399</v>
@@ -1208,10 +1208,10 @@
         <v>14140.33527193919</v>
       </c>
       <c r="G12">
-        <v>59001.16008174044</v>
+        <v>60659.45806046302</v>
       </c>
       <c r="H12">
-        <v>3.009366656605827</v>
+        <v>3.295288861825552</v>
       </c>
       <c r="I12">
         <v>43862.5</v>
@@ -1222,10 +1222,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-12679.31801457126</v>
+        <v>-10843.62591971395</v>
       </c>
       <c r="C13">
-        <v>-465.9552499247848</v>
+        <v>-288.5611337900527</v>
       </c>
       <c r="D13">
         <v>180289.2747172246</v>
@@ -1237,10 +1237,10 @@
         <v>14423.14197737797</v>
       </c>
       <c r="G13">
-        <v>64143.2500971147</v>
+        <v>65978.94219197202</v>
       </c>
       <c r="H13">
-        <v>3.515464338428131</v>
+        <v>3.781339006911555</v>
       </c>
       <c r="I13">
         <v>43862.5</v>
@@ -1251,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-13051.11738293954</v>
+        <v>-11033.59631904412</v>
       </c>
       <c r="C14">
-        <v>-371.7993683682762</v>
+        <v>-189.9703993301763</v>
       </c>
       <c r="D14">
         <v>183895.0602115691</v>
@@ -1266,10 +1266,10 @@
         <v>14711.60481692553</v>
       </c>
       <c r="G14">
-        <v>69617.98126637889</v>
+        <v>71635.50233027429</v>
       </c>
       <c r="H14">
-        <v>3.924753652879165</v>
+        <v>4.172457787069916</v>
       </c>
       <c r="I14">
         <v>43862.5</v>
@@ -1280,10 +1280,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-13323.26880892929</v>
+        <v>-11119.37305176982</v>
       </c>
       <c r="C15">
-        <v>-272.1514259897477</v>
+        <v>-85.77673272569882</v>
       </c>
       <c r="D15">
         <v>187572.9614158005</v>
@@ -1295,10 +1295,10 @@
         <v>15005.83691326404</v>
       </c>
       <c r="G15">
-        <v>75444.91578890859</v>
+        <v>77648.81154606806</v>
       </c>
       <c r="H15">
-        <v>4.260115033245682</v>
+        <v>4.491294651569389</v>
       </c>
       <c r="I15">
         <v>43862.5</v>
@@ -1309,10 +1309,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-13490.16140364661</v>
+        <v>-11095.23158589149</v>
       </c>
       <c r="C16">
-        <v>-166.8925947173238</v>
+        <v>24.14146587832965</v>
       </c>
       <c r="D16">
         <v>191324.4206441165</v>
@@ -1324,10 +1324,10 @@
         <v>15305.95365152932</v>
       </c>
       <c r="G16">
-        <v>81644.70082470181</v>
+        <v>84039.63064245693</v>
       </c>
       <c r="H16">
-        <v>4.537931271998419</v>
+        <v>4.75403684827842</v>
       </c>
       <c r="I16">
         <v>43862.5</v>
@@ -1338,10 +1338,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-13546.0632183619</v>
+        <v>-10955.32348849623</v>
       </c>
       <c r="C17">
-        <v>-55.90181471528558</v>
+        <v>139.9080973952632</v>
       </c>
       <c r="D17">
         <v>195150.9090569989</v>
@@ -1353,10 +1353,10 @@
         <v>15612.07272455991</v>
       </c>
       <c r="G17">
-        <v>88239.14046094843</v>
+        <v>90829.8801908141</v>
       </c>
       <c r="H17">
-        <v>4.770220802404679</v>
+        <v>4.972536327405597</v>
       </c>
       <c r="I17">
         <v>43862.5</v>
@@ -1367,10 +1367,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-13485.11898650937</v>
+        <v>-10693.6740967304</v>
       </c>
       <c r="C18">
-        <v>60.94423185252617</v>
+        <v>261.6493917658336</v>
       </c>
       <c r="D18">
         <v>199053.9272381389</v>
@@ -1382,10 +1382,10 @@
         <v>15924.31417905111</v>
       </c>
       <c r="G18">
-        <v>95251.27281104775</v>
+        <v>98042.71770082673</v>
       </c>
       <c r="H18">
-        <v>4.965985570625864</v>
+        <v>5.1556524844107</v>
       </c>
       <c r="I18">
         <v>43862.5</v>
@@ -1396,10 +1396,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-13301.34783997649</v>
+        <v>-10304.18016128637</v>
       </c>
       <c r="C19">
-        <v>183.771146532883</v>
+        <v>389.493935444023</v>
       </c>
       <c r="D19">
         <v>203035.0057829016</v>
@@ -1411,10 +1411,10 @@
         <v>16242.80046263213</v>
       </c>
       <c r="G19">
-        <v>102705.4526209273</v>
+        <v>105702.6202996174</v>
       </c>
       <c r="H19">
-        <v>5.132090723338067</v>
+        <v>5.310127733379844</v>
       </c>
       <c r="I19">
         <v>43862.5</v>
@@ -1425,10 +1425,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-12988.64100026996</v>
+        <v>-9780.607462945929</v>
       </c>
       <c r="C20">
-        <v>312.7068397065268</v>
+        <v>523.5726983404439</v>
       </c>
       <c r="D20">
         <v>207095.7058985597</v>
@@ -1440,10 +1440,10 @@
         <v>16567.65647188477</v>
       </c>
       <c r="G20">
-        <v>110627.4397850791</v>
+        <v>113835.4733224032</v>
       </c>
       <c r="H20">
-        <v>5.273855033289565</v>
+        <v>5.441174624457368</v>
       </c>
       <c r="I20">
         <v>43862.5</v>
@@ -1454,10 +1454,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-12540.75944520912</v>
+        <v>-9116.588402785315</v>
       </c>
       <c r="C21">
-        <v>447.881555060847</v>
+        <v>664.0190601606137</v>
       </c>
       <c r="D21">
         <v>211237.6200165309</v>
@@ -1469,10 +1469,10 @@
         <v>16899.00960132247</v>
       </c>
       <c r="G21">
-        <v>119044.4942043279</v>
+        <v>122468.6652467517</v>
       </c>
       <c r="H21">
-        <v>5.395456974760782</v>
+        <v>5.552879246791598</v>
       </c>
       <c r="I21">
         <v>43862.5</v>
@@ -1483,10 +1483,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-11951.33155186471</v>
+        <v>-8305.619566713654</v>
       </c>
       <c r="C22">
-        <v>589.4278933444037</v>
+        <v>810.9688360716609</v>
       </c>
       <c r="D22">
         <v>215462.3724168615</v>
@@ -1498,10 +1498,10 @@
         <v>17236.98979334892</v>
       </c>
       <c r="G22">
-        <v>127985.4774491168</v>
+        <v>131631.1894342678</v>
       </c>
       <c r="H22">
-        <v>5.500220076310836</v>
+        <v>5.648484409863364</v>
       </c>
       <c r="I22">
         <v>43862.5</v>
@@ -1512,10 +1512,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-11213.85071653245</v>
+        <v>-7341.059265085951</v>
       </c>
       <c r="C23">
-        <v>737.4808353322605</v>
+        <v>964.5603016277037</v>
       </c>
       <c r="D23">
         <v>219771.6198651987</v>
@@ -1527,10 +1527,10 @@
         <v>17581.7295892159</v>
       </c>
       <c r="G23">
-        <v>137480.9617262163</v>
+        <v>141353.7531776628</v>
       </c>
       <c r="H23">
-        <v>5.590817299935957</v>
+        <v>5.730592247577526</v>
       </c>
       <c r="I23">
         <v>43862.5</v>
@@ -1541,10 +1541,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-10321.67295260555</v>
+        <v>-6216.125048206222</v>
       </c>
       <c r="C24">
-        <v>892.1777639269003</v>
+        <v>1124.934216879728</v>
       </c>
       <c r="D24">
         <v>224167.0522625027</v>
@@ -1556,10 +1556,10 @@
         <v>17933.36418100022</v>
       </c>
       <c r="G24">
-        <v>147563.3466833866</v>
+        <v>151668.8945877859</v>
       </c>
       <c r="H24">
-        <v>5.669419938079145</v>
+        <v>5.80131165526776</v>
       </c>
       <c r="I24">
         <v>43862.5</v>
@@ -1570,10 +1570,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-9268.014467289775</v>
+        <v>-4923.891198613792</v>
       </c>
       <c r="C25">
-        <v>1053.658485315776</v>
+        <v>1292.23384959243</v>
       </c>
       <c r="D25">
         <v>228650.3933077528</v>
@@ -1585,10 +1585,10 @@
         <v>18292.03146462022</v>
       </c>
       <c r="G25">
-        <v>158266.9846258519</v>
+        <v>162611.1078945278</v>
       </c>
       <c r="H25">
-        <v>5.737807762765801</v>
+        <v>5.862367230714871</v>
       </c>
       <c r="I25">
         <v>43862.5</v>
@@ -1599,10 +1599,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-8045.949218187843</v>
+        <v>-3457.286201128296</v>
       </c>
       <c r="C26">
-        <v>1222.065249101932</v>
+        <v>1466.604997485495</v>
       </c>
       <c r="D26">
         <v>233223.4011739078</v>
@@ -1614,10 +1614,10 @@
         <v>18657.87209391263</v>
       </c>
       <c r="G26">
-        <v>169628.3147606672</v>
+        <v>174216.9777777268</v>
       </c>
       <c r="H26">
-        <v>5.79745164498966</v>
+        <v>5.915180888017191</v>
       </c>
       <c r="I26">
         <v>43862.5</v>
@@ -1628,10 +1628,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-6648.406450868057</v>
+        <v>-1809.090191715356</v>
       </c>
       <c r="C27">
-        <v>1397.542767319787</v>
+        <v>1648.196009412941</v>
       </c>
       <c r="D27">
         <v>237887.869197386</v>
@@ -1643,10 +1643,10 @@
         <v>19031.02953579088</v>
       </c>
       <c r="G27">
-        <v>181686.007130392</v>
+        <v>186525.3233895447</v>
       </c>
       <c r="H27">
-        <v>5.849576308142423</v>
+        <v>5.960933769460341</v>
       </c>
       <c r="I27">
         <v>43862.5</v>
@@ -1657,10 +1657,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-5068.168218624437</v>
+        <v>28.06761367374929</v>
       </c>
       <c r="C28">
-        <v>1580.23823224362</v>
+        <v>1837.157805389105</v>
       </c>
       <c r="D28">
         <v>242645.6265813337</v>
@@ -1672,10 +1672,10 @@
         <v>19411.6501265067</v>
       </c>
       <c r="G28">
-        <v>194481.116946155</v>
+        <v>199577.3527784532</v>
       </c>
       <c r="H28">
-        <v>5.895208541623909</v>
+        <v>6.00061375104548</v>
       </c>
       <c r="I28">
         <v>43862.5</v>
@@ -1686,10 +1686,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-3297.866885733338</v>
+        <v>2061.711509038969</v>
       </c>
       <c r="C29">
-        <v>1770.301332891099</v>
+        <v>2033.64389536522</v>
       </c>
       <c r="D29">
         <v>247498.5391129604</v>
@@ -1701,10 +1701,10 @@
         <v>19799.88312903683</v>
       </c>
       <c r="G29">
-        <v>208057.2500824542</v>
+        <v>213416.8284772265</v>
       </c>
       <c r="H29">
-        <v>5.935214634417973</v>
+        <v>6.035052277284403</v>
       </c>
       <c r="I29">
         <v>43862.5</v>
@@ -1715,10 +1715,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>-1329.982615613986</v>
+        <v>4299.521905694288</v>
       </c>
       <c r="C30">
-        <v>1967.884270119352</v>
+        <v>2237.810396655319</v>
       </c>
       <c r="D30">
         <v>252448.5098952196</v>
@@ -1730,10 +1730,10 @@
         <v>20195.88079161757</v>
       </c>
       <c r="G30">
-        <v>222460.74055214</v>
+        <v>228090.2450734483</v>
       </c>
       <c r="H30">
-        <v>5.970329720905032</v>
+        <v>6.064953198237122</v>
       </c>
       <c r="I30">
         <v>43862.5</v>
@@ -1744,10 +1744,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>843.1591545914707</v>
+        <v>6749.337955599123</v>
       </c>
       <c r="C31">
-        <v>2173.141770205457</v>
+        <v>2449.816049904835</v>
       </c>
       <c r="D31">
         <v>257497.480093124</v>
@@ -1759,10 +1759,10 @@
         <v>20599.79840744992</v>
       </c>
       <c r="G31">
-        <v>237740.8408402685</v>
+        <v>243647.0196412762</v>
       </c>
       <c r="H31">
-        <v>6.001180992228905</v>
+        <v>6.090915546620179</v>
       </c>
       <c r="I31">
         <v>43862.5</v>

</xml_diff>

<commit_message>
Added documentation exec summary and cover page
</commit_message>
<xml_diff>
--- a/317 Newell St/Results/Excels/Performance_KPIs.xlsx
+++ b/317 Newell St/Results/Excels/Performance_KPIs.xlsx
@@ -427,10 +427,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-7.852283465351582</v>
+        <v>-8.201936737888872</v>
       </c>
       <c r="C2">
-        <v>-3444.207834989838</v>
+        <v>-3597.574501656507</v>
       </c>
       <c r="D2">
         <v>43862.5</v>
@@ -441,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-1.952164101635395</v>
+        <v>-2.480156882104665</v>
       </c>
       <c r="C3">
-        <v>-856.2679790798252</v>
+        <v>-1087.858812413159</v>
       </c>
       <c r="D3">
         <v>43862.5</v>
@@ -455,10 +455,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-2.158498741133831</v>
+        <v>-2.692992376547527</v>
       </c>
       <c r="C4">
-        <v>-946.7715103298265</v>
+        <v>-1181.213781163159</v>
       </c>
       <c r="D4">
         <v>43862.5</v>
@@ -469,10 +469,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-2.037905112250963</v>
+        <v>-2.585761088550001</v>
       </c>
       <c r="C5">
-        <v>-893.8761298610789</v>
+        <v>-1134.179457465244</v>
       </c>
       <c r="D5">
         <v>43862.5</v>
@@ -483,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-1.906826571400646</v>
+        <v>-2.468378947107166</v>
       </c>
       <c r="C6">
-        <v>-836.3818048806086</v>
+        <v>-1082.692715674881</v>
       </c>
       <c r="D6">
         <v>43862.5</v>
@@ -497,10 +497,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-1.765030491594487</v>
+        <v>-2.34062167669367</v>
       </c>
       <c r="C7">
-        <v>-774.1864993756319</v>
+        <v>-1026.655182939761</v>
       </c>
       <c r="D7">
         <v>43862.5</v>
@@ -511,10 +511,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-1.612279610001771</v>
+        <v>-2.202260574728433</v>
       </c>
       <c r="C8">
-        <v>-707.1861439370266</v>
+        <v>-965.9665445902588</v>
       </c>
       <c r="D8">
         <v>43862.5</v>
@@ -525,10 +525,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1.448331959246771</v>
+        <v>-2.0530624480916</v>
       </c>
       <c r="C9">
-        <v>-635.2746056246151</v>
+        <v>-900.5245162941778</v>
       </c>
       <c r="D9">
         <v>43862.5</v>
@@ -539,10 +539,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-1.272940798876131</v>
+        <v>-1.892789549942089</v>
       </c>
       <c r="C10">
-        <v>-558.3436579070431</v>
+        <v>-830.2248163433489</v>
       </c>
       <c r="D10">
         <v>43862.5</v>
@@ -553,10 +553,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-1.085854547076172</v>
+        <v>-1.721199516918767</v>
       </c>
       <c r="C11">
-        <v>-476.2829507112858</v>
+        <v>-754.9611381084942</v>
       </c>
       <c r="D11">
         <v>43862.5</v>
@@ -567,10 +567,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.8868167127249336</v>
+        <v>-1.53804530681359</v>
       </c>
       <c r="C12">
-        <v>-388.979980618974</v>
+        <v>-674.6251227011106</v>
       </c>
       <c r="D12">
         <v>43862.5</v>
@@ -581,10 +581,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.675565827868966</v>
+        <v>-1.343075136809851</v>
       </c>
       <c r="C13">
-        <v>-296.3200612490252</v>
+        <v>-589.1063318832207</v>
       </c>
       <c r="D13">
         <v>43862.5</v>
@@ -595,10 +595,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-0.4518353807204318</v>
+        <v>-1.136032422384842</v>
       </c>
       <c r="C14">
-        <v>-198.1862938684994</v>
+        <v>-498.2922212685514</v>
       </c>
       <c r="D14">
         <v>43862.5</v>
@@ -609,10 +609,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.2153537492757411</v>
+        <v>-0.9166557169817396</v>
       </c>
       <c r="C15">
-        <v>-94.45953827607195</v>
+        <v>-402.0681138611155</v>
       </c>
       <c r="D15">
         <v>43862.5</v>
@@ -623,10 +623,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0.03415586433664432</v>
+        <v>-0.68467865256201</v>
       </c>
       <c r="C16">
-        <v>14.98161599466062</v>
+        <v>-300.3171739800116</v>
       </c>
       <c r="D16">
         <v>43862.5</v>
@@ -637,10 +637,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.2969754986655694</v>
+        <v>-0.4398298811555597</v>
       </c>
       <c r="C17">
-        <v>130.2608781021854</v>
+        <v>-192.9203816218574</v>
       </c>
       <c r="D17">
         <v>43862.5</v>
@@ -651,10 +651,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0.5733924967834013</v>
+        <v>-0.1818330175332416</v>
       </c>
       <c r="C18">
-        <v>251.5042839016194</v>
+        <v>-79.75650731551809</v>
       </c>
       <c r="D18">
         <v>43862.5</v>
@@ -665,10 +665,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0.8636995690415287</v>
+        <v>0.08959341686695485</v>
       </c>
       <c r="C19">
-        <v>378.8402234708405</v>
+        <v>39.29791247326807</v>
       </c>
       <c r="D19">
         <v>43862.5</v>
@@ -679,10 +679,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1.168194854600343</v>
+        <v>0.3747360486214085</v>
       </c>
       <c r="C20">
-        <v>512.3994680990755</v>
+        <v>164.3685993265653</v>
       </c>
       <c r="D20">
         <v>43862.5</v>
@@ -693,10 +693,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1.487181981591563</v>
+        <v>0.6738867054631527</v>
       </c>
       <c r="C21">
-        <v>652.3151966755995</v>
+        <v>295.5835561837753</v>
       </c>
       <c r="D21">
         <v>43862.5</v>
@@ -707,10 +707,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1.820970125762113</v>
+        <v>0.9873424677305062</v>
       </c>
       <c r="C22">
-        <v>798.723021412407</v>
+        <v>433.0730899082932</v>
       </c>
       <c r="D22">
         <v>43862.5</v>
@@ -721,10 +721,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2.169874067441133</v>
+        <v>1.315405717958728</v>
       </c>
       <c r="C23">
-        <v>951.7610128313668</v>
+        <v>576.9698330396471</v>
       </c>
       <c r="D23">
         <v>43862.5</v>
@@ -735,10 +735,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2.534214246661863</v>
+        <v>1.658384188442401</v>
       </c>
       <c r="C24">
-        <v>1111.56972394206</v>
+        <v>727.4087646555481</v>
       </c>
       <c r="D24">
         <v>43862.5</v>
@@ -749,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2.91431681626227</v>
+        <v>2.016591006587315</v>
       </c>
       <c r="C25">
-        <v>1278.292213533038</v>
+        <v>884.5272302643612</v>
       </c>
       <c r="D25">
         <v>43862.5</v>
@@ -763,10 +763,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>3.310513692777216</v>
+        <v>2.390344737860391</v>
       </c>
       <c r="C26">
-        <v>1452.074068494407</v>
+        <v>1048.464960644014</v>
       </c>
       <c r="D26">
         <v>43862.5</v>
@@ -777,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3.72314260492597</v>
+        <v>2.779969426136218</v>
       </c>
       <c r="C27">
-        <v>1633.063425085654</v>
+        <v>1219.364089538999</v>
       </c>
       <c r="D27">
         <v>43862.5</v>
@@ -791,10 +791,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>4.152547139487621</v>
+        <v>3.185794631228124</v>
       </c>
       <c r="C28">
-        <v>1821.410989057758</v>
+        <v>1397.369170122436</v>
       </c>
       <c r="D28">
         <v>43862.5</v>
@@ -805,10 +805,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4.599076784346256</v>
+        <v>3.608155463380283</v>
       </c>
       <c r="C29">
-        <v>2017.270054533877</v>
+        <v>1582.627190125177</v>
       </c>
       <c r="D29">
         <v>43862.5</v>
@@ -819,10 +819,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>5.063086968476059</v>
+        <v>4.047392614485933</v>
       </c>
       <c r="C30">
-        <v>2220.796521547811</v>
+        <v>1775.287585528892</v>
       </c>
       <c r="D30">
         <v>43862.5</v>
@@ -833,10 +833,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>5.544939098624205</v>
+        <v>4.503852385784318</v>
       </c>
       <c r="C31">
-        <v>2432.148912134042</v>
+        <v>1975.502252714647</v>
       </c>
       <c r="D31">
         <v>43862.5</v>
@@ -847,10 +847,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0.4528956112671862</v>
+        <v>0.3659616902357496</v>
       </c>
       <c r="C32">
-        <v>198.6513374920696</v>
+        <v>160.5199463796557</v>
       </c>
       <c r="D32">
         <v>43862.5</v>
@@ -903,10 +903,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-3397.126729079823</v>
+        <v>-3571.993395746492</v>
       </c>
       <c r="C2">
-        <v>-3397.126729079823</v>
+        <v>-3571.993395746492</v>
       </c>
       <c r="D2">
         <v>145000</v>
@@ -918,7 +918,7 @@
         <v>11600</v>
       </c>
       <c r="G2">
-        <v>22331.22580205838</v>
+        <v>22156.35913539171</v>
       </c>
       <c r="H2">
         <v>-100</v>
@@ -932,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-4388.598458159649</v>
+        <v>-4792.655124826318</v>
       </c>
       <c r="C3">
-        <v>-991.4717290798253</v>
+        <v>-1220.661729079825</v>
       </c>
       <c r="D3">
         <v>147900</v>
@@ -947,10 +947,10 @@
         <v>11832</v>
       </c>
       <c r="G3">
-        <v>25165.49861547235</v>
+        <v>24761.44194880568</v>
       </c>
       <c r="H3">
-        <v>-42.62639244121436</v>
+        <v>-43.5475817639084</v>
       </c>
       <c r="I3">
         <v>43862.5</v>
@@ -961,10 +961,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-5331.306312239475</v>
+        <v>-5970.282728906143</v>
       </c>
       <c r="C4">
-        <v>-942.7078540798266</v>
+        <v>-1177.627604079826</v>
       </c>
       <c r="D4">
         <v>150858</v>
@@ -976,10 +976,10 @@
         <v>12068.64</v>
       </c>
       <c r="G4">
-        <v>28187.13242737833</v>
+        <v>27548.15601071166</v>
       </c>
       <c r="H4">
-        <v>-19.83611481913701</v>
+        <v>-20.74994426938493</v>
       </c>
       <c r="I4">
         <v>43862.5</v>
@@ -990,10 +990,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-6220.743194444304</v>
+        <v>-7100.512354860971</v>
       </c>
       <c r="C5">
-        <v>-889.4368822048291</v>
+        <v>-1130.229625954827</v>
       </c>
       <c r="D5">
         <v>153875.16</v>
@@ -1005,10 +1005,10 @@
         <v>12310.0128</v>
       </c>
       <c r="G5">
-        <v>31407.9769839877</v>
+        <v>30528.20782357103</v>
       </c>
       <c r="H5">
-        <v>-10.5358868994265</v>
+        <v>-11.37913675955493</v>
       </c>
       <c r="I5">
         <v>43862.5</v>
@@ -1019,10 +1019,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-7052.301810477256</v>
+        <v>-8178.883533237675</v>
       </c>
       <c r="C6">
-        <v>-831.5586160329522</v>
+        <v>-1078.371178376704</v>
       </c>
       <c r="D6">
         <v>156952.6632</v>
@@ -1034,10 +1034,10 @@
         <v>12556.213056</v>
       </c>
       <c r="G6">
-        <v>34840.46559303495</v>
+        <v>33713.88387027453</v>
       </c>
       <c r="H6">
-        <v>-5.594424899848416</v>
+        <v>-6.367018772471189</v>
       </c>
       <c r="I6">
         <v>43862.5</v>
@@ -1048,10 +1048,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-7821.272662884041</v>
+        <v>-9200.837262046804</v>
       </c>
       <c r="C7">
-        <v>-768.9708524067846</v>
+        <v>-1021.95372880913</v>
       </c>
       <c r="D7">
         <v>160091.716464</v>
@@ -1063,10 +1063,10 @@
         <v>12807.33731712</v>
       </c>
       <c r="G7">
-        <v>38497.65157189648</v>
+        <v>37118.08697273372</v>
       </c>
       <c r="H7">
-        <v>-2.57550321425799</v>
+        <v>-3.283974572695414</v>
       </c>
       <c r="I7">
         <v>43862.5</v>
@@ -1077,10 +1077,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-8522.842015142</v>
+        <v>-10161.71406261716</v>
       </c>
       <c r="C8">
-        <v>-701.5693522579577</v>
+        <v>-960.8768005703614</v>
       </c>
       <c r="D8">
         <v>163293.55079328</v>
@@ -1092,10 +1092,10 @@
         <v>13063.4840634624</v>
       </c>
       <c r="G8">
-        <v>42393.24723876181</v>
+        <v>40754.37519128665</v>
       </c>
       <c r="H8">
-        <v>-0.5662350551105422</v>
+        <v>-1.217470459994541</v>
       </c>
       <c r="I8">
         <v>43862.5</v>
@@ -1106,10 +1106,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-9152.089825618128</v>
+        <v>-11056.75200761351</v>
       </c>
       <c r="C9">
-        <v>-629.2478104761294</v>
+        <v>-895.037944996343</v>
       </c>
       <c r="D9">
         <v>166559.4218091457</v>
@@ -1121,10 +1121,10 @@
         <v>13324.75374473165</v>
       </c>
       <c r="G9">
-        <v>46541.66563136013</v>
+        <v>44637.00344936474</v>
       </c>
       <c r="H9">
-        <v>0.8505713411053994</v>
+        <v>0.2503621393163291</v>
       </c>
       <c r="I9">
         <v>43862.5</v>
@@ -1135,10 +1135,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-9703.987651473435</v>
+        <v>-11881.08472135204</v>
       </c>
       <c r="C10">
-        <v>-551.8978258553079</v>
+        <v>-824.3327137385313</v>
       </c>
       <c r="D10">
         <v>169890.6102453286</v>
@@ -1150,10 +1150,10 @@
         <v>13591.24881962629</v>
       </c>
       <c r="G10">
-        <v>50958.06515129079</v>
+        <v>48780.96808141219</v>
       </c>
       <c r="H10">
-        <v>1.891966364283193</v>
+        <v>1.337370072019706</v>
       </c>
       <c r="I10">
         <v>43862.5</v>
@@ -1164,10 +1164,10 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-10173.39652262617</v>
+        <v>-12629.73935258507</v>
       </c>
       <c r="C11">
-        <v>-469.4088711527384</v>
+        <v>-748.6546312330363</v>
       </c>
       <c r="D11">
         <v>173288.4224502351</v>
@@ -1179,10 +1179,10 @@
         <v>13863.07379601881</v>
       </c>
       <c r="G11">
-        <v>55658.39734655086</v>
+        <v>53202.05451659196</v>
       </c>
       <c r="H11">
-        <v>2.681696413227197</v>
+        <v>2.16802602528845</v>
       </c>
       <c r="I11">
         <v>43862.5</v>
@@ -1193,10 +1193,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-10555.0647859239</v>
+        <v>-13297.6345199651</v>
       </c>
       <c r="C12">
-        <v>-381.6682632977227</v>
+        <v>-667.8951673800265</v>
       </c>
       <c r="D12">
         <v>176754.1908992399</v>
@@ -1208,10 +1208,10 @@
         <v>14140.33527193919</v>
       </c>
       <c r="G12">
-        <v>60659.45806046302</v>
+        <v>57916.88832642182</v>
       </c>
       <c r="H12">
-        <v>3.295288861825552</v>
+        <v>2.818481109824966</v>
       </c>
       <c r="I12">
         <v>43862.5</v>
@@ -1222,10 +1222,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-10843.62591971395</v>
+        <v>-13879.57823043952</v>
       </c>
       <c r="C13">
-        <v>-288.5611337900527</v>
+        <v>-581.9437104744202</v>
       </c>
       <c r="D13">
         <v>180289.2747172246</v>
@@ -1237,10 +1237,10 @@
         <v>14423.14197737797</v>
       </c>
       <c r="G13">
-        <v>65978.94219197202</v>
+        <v>62942.98988124645</v>
       </c>
       <c r="H13">
-        <v>3.781339006911555</v>
+        <v>3.337857574437986</v>
       </c>
       <c r="I13">
         <v>43862.5</v>
@@ -1251,10 +1251,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-11033.59631904412</v>
+        <v>-14370.26577087118</v>
       </c>
       <c r="C14">
-        <v>-189.9703993301763</v>
+        <v>-490.6875404316543</v>
       </c>
       <c r="D14">
         <v>183895.0602115691</v>
@@ -1266,10 +1266,10 @@
         <v>14711.60481692553</v>
       </c>
       <c r="G14">
-        <v>71635.50233027429</v>
+        <v>68298.83287844725</v>
       </c>
       <c r="H14">
-        <v>4.172457787069916</v>
+        <v>3.759210468235108</v>
       </c>
       <c r="I14">
         <v>43862.5</v>
@@ -1280,10 +1280,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-11119.37305176982</v>
+        <v>-14764.27757322588</v>
       </c>
       <c r="C15">
-        <v>-85.77673272569882</v>
+        <v>-394.0118023547029</v>
       </c>
       <c r="D15">
         <v>187572.9614158005</v>
@@ -1295,10 +1295,10 @@
         <v>15005.83691326404</v>
       </c>
       <c r="G15">
-        <v>77648.81154606806</v>
+        <v>74003.90702461201</v>
       </c>
       <c r="H15">
-        <v>4.491294651569389</v>
+        <v>4.105564560408226</v>
       </c>
       <c r="I15">
         <v>43862.5</v>
@@ -1309,10 +1309,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-11095.23158589149</v>
+        <v>-15056.07705371728</v>
       </c>
       <c r="C16">
-        <v>24.14146587832965</v>
+        <v>-291.7994804914033</v>
       </c>
       <c r="D16">
         <v>191324.4206441165</v>
@@ -1324,10 +1324,10 @@
         <v>15305.95365152932</v>
       </c>
       <c r="G16">
-        <v>84039.63064245693</v>
+        <v>80078.78517463114</v>
       </c>
       <c r="H16">
-        <v>4.75403684827842</v>
+        <v>4.393425776506388</v>
       </c>
       <c r="I16">
         <v>43862.5</v>
@@ -1338,10 +1338,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-10955.32348849623</v>
+        <v>-15240.008426351</v>
       </c>
       <c r="C17">
-        <v>139.9080973952632</v>
+        <v>-183.9313726337168</v>
       </c>
       <c r="D17">
         <v>195150.9090569989</v>
@@ -1353,10 +1353,10 @@
         <v>15612.07272455991</v>
       </c>
       <c r="G17">
-        <v>90829.8801908141</v>
+        <v>86545.19525295934</v>
       </c>
       <c r="H17">
-        <v>4.972536327405597</v>
+        <v>4.634918102108165</v>
       </c>
       <c r="I17">
         <v>43862.5</v>
@@ -1367,10 +1367,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-10693.6740967304</v>
+        <v>-15310.29449136486</v>
       </c>
       <c r="C18">
-        <v>261.6493917658336</v>
+        <v>-70.28606501386366</v>
       </c>
       <c r="D18">
         <v>199053.9272381389</v>
@@ -1382,10 +1382,10 @@
         <v>15924.31417905111</v>
       </c>
       <c r="G18">
-        <v>98042.71770082673</v>
+        <v>93426.09730619227</v>
       </c>
       <c r="H18">
-        <v>5.1556524844107</v>
+        <v>4.839134419868896</v>
       </c>
       <c r="I18">
         <v>43862.5</v>
@@ -1396,10 +1396,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-10304.18016128637</v>
+        <v>-15261.03439912004</v>
       </c>
       <c r="C19">
-        <v>389.493935444023</v>
+        <v>49.2600922448255</v>
       </c>
       <c r="D19">
         <v>203035.0057829016</v>
@@ -1411,10 +1411,10 @@
         <v>16242.80046263213</v>
       </c>
       <c r="G19">
-        <v>105702.6202996174</v>
+        <v>100745.7660617837</v>
       </c>
       <c r="H19">
-        <v>5.310127733379844</v>
+        <v>5.01301860788943</v>
       </c>
       <c r="I19">
         <v>43862.5</v>
@@ -1425,10 +1425,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-9780.607462945929</v>
+        <v>-15086.20139005877</v>
       </c>
       <c r="C20">
-        <v>523.5726983404439</v>
+        <v>174.8330090612689</v>
       </c>
       <c r="D20">
         <v>207095.7058985597</v>
@@ -1440,10 +1440,10 @@
         <v>16567.65647188477</v>
       </c>
       <c r="G20">
-        <v>113835.4733224032</v>
+        <v>108529.8793952903</v>
       </c>
       <c r="H20">
-        <v>5.441174624457368</v>
+        <v>5.161957925469496</v>
       </c>
       <c r="I20">
         <v>43862.5</v>
@@ -1454,10 +1454,10 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-9116.588402785315</v>
+        <v>-14779.64051140931</v>
       </c>
       <c r="C21">
-        <v>664.0190601606137</v>
+        <v>306.5608786494577</v>
       </c>
       <c r="D21">
         <v>211237.6200165309</v>
@@ -1469,10 +1469,10 @@
         <v>16899.00960132247</v>
       </c>
       <c r="G21">
-        <v>122468.6652467517</v>
+        <v>116805.6131381277</v>
       </c>
       <c r="H21">
-        <v>5.552879246791598</v>
+        <v>5.290190687503293</v>
       </c>
       <c r="I21">
         <v>43862.5</v>
@@ -1483,10 +1483,10 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-8305.619566713654</v>
+        <v>-14335.06631138658</v>
       </c>
       <c r="C22">
-        <v>810.9688360716609</v>
+        <v>444.5742000227328</v>
       </c>
       <c r="D22">
         <v>215462.3724168615</v>
@@ -1498,10 +1498,10 @@
         <v>17236.98979334892</v>
       </c>
       <c r="G22">
-        <v>131631.1894342678</v>
+        <v>125601.7426895949</v>
       </c>
       <c r="H22">
-        <v>5.648484409863364</v>
+        <v>5.401092927579509</v>
       </c>
       <c r="I22">
         <v>43862.5</v>
@@ -1512,10 +1512,10 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-7341.059265085951</v>
+        <v>-13746.06051170903</v>
       </c>
       <c r="C23">
-        <v>964.5603016277037</v>
+        <v>589.0057996775485</v>
       </c>
       <c r="D23">
         <v>219771.6198651987</v>
@@ -1527,10 +1527,10 @@
         <v>17581.7295892159</v>
       </c>
       <c r="G23">
-        <v>141353.7531776628</v>
+        <v>134948.7519310397</v>
       </c>
       <c r="H23">
-        <v>5.730592247577526</v>
+        <v>5.497383856713944</v>
       </c>
       <c r="I23">
         <v>43862.5</v>
@@ -1541,10 +1541,10 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>-6216.125048206222</v>
+        <v>-13006.06965932821</v>
       </c>
       <c r="C24">
-        <v>1124.934216879728</v>
+        <v>739.9908523808208</v>
       </c>
       <c r="D24">
         <v>224167.0522625027</v>
@@ -1556,10 +1556,10 @@
         <v>17933.36418100022</v>
       </c>
       <c r="G24">
-        <v>151668.8945877859</v>
+        <v>144878.9499766639</v>
       </c>
       <c r="H24">
-        <v>5.80131165526776</v>
+        <v>5.58127565472808</v>
       </c>
       <c r="I24">
         <v>43862.5</v>
@@ -1570,10 +1570,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-4923.891198613792</v>
+        <v>-12108.40275834716</v>
       </c>
       <c r="C25">
-        <v>1292.23384959243</v>
+        <v>897.6669009810466</v>
       </c>
       <c r="D25">
         <v>228650.3933077528</v>
@@ -1585,10 +1585,10 @@
         <v>18292.03146462022</v>
       </c>
       <c r="G25">
-        <v>162611.1078945278</v>
+        <v>155426.5963347945</v>
       </c>
       <c r="H25">
-        <v>5.862367230714871</v>
+        <v>5.654584364416904</v>
       </c>
       <c r="I25">
         <v>43862.5</v>
@@ -1599,10 +1599,10 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-3457.286201128296</v>
+        <v>-11046.22888318833</v>
       </c>
       <c r="C26">
-        <v>1466.604997485495</v>
+        <v>1062.173875158829</v>
       </c>
       <c r="D26">
         <v>233223.4011739078</v>
@@ -1614,10 +1614,10 @@
         <v>18657.87209391263</v>
       </c>
       <c r="G26">
-        <v>174216.9777777268</v>
+        <v>166628.0350956667</v>
       </c>
       <c r="H26">
-        <v>5.915180888017191</v>
+        <v>5.718813134913003</v>
       </c>
       <c r="I26">
         <v>43862.5</v>
@@ -1628,10 +1628,10 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-1809.090191715356</v>
+        <v>-9812.574774160226</v>
       </c>
       <c r="C27">
-        <v>1648.196009412941</v>
+        <v>1233.654109028105</v>
       </c>
       <c r="D27">
         <v>237887.869197386</v>
@@ -1643,10 +1643,10 @@
         <v>19031.02953579088</v>
       </c>
       <c r="G27">
-        <v>186525.3233895447</v>
+        <v>178521.8388070998</v>
       </c>
       <c r="H27">
-        <v>5.960933769460341</v>
+        <v>5.775215500424702</v>
       </c>
       <c r="I27">
         <v>43862.5</v>
@@ -1657,10 +1657,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>28.06761367374929</v>
+        <v>-8400.322416665578</v>
       </c>
       <c r="C28">
-        <v>1837.157805389105</v>
+        <v>1412.252357494648</v>
       </c>
       <c r="D28">
         <v>242645.6265813337</v>
@@ -1672,10 +1672,10 @@
         <v>19411.6501265067</v>
       </c>
       <c r="G28">
-        <v>199577.3527784532</v>
+        <v>191148.9627481138</v>
       </c>
       <c r="H28">
-        <v>6.00061375104548</v>
+        <v>5.824844038284493</v>
       </c>
       <c r="I28">
         <v>43862.5</v>
@@ -1686,10 +1686,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2061.711509038969</v>
+        <v>-6802.206605392172</v>
       </c>
       <c r="C29">
-        <v>2033.64389536522</v>
+        <v>1598.115811273407</v>
       </c>
       <c r="D29">
         <v>247498.5391129604</v>
@@ -1701,10 +1701,10 @@
         <v>19799.88312903683</v>
       </c>
       <c r="G29">
-        <v>213416.8284772265</v>
+        <v>204552.9103627954</v>
       </c>
       <c r="H29">
-        <v>6.035052277284403</v>
+        <v>5.868588180321543</v>
       </c>
       <c r="I29">
         <v>43862.5</v>
@@ -1715,10 +1715,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4299.521905694288</v>
+        <v>-5010.812494930962</v>
       </c>
       <c r="C30">
-        <v>2237.810396655319</v>
+        <v>1791.394110461209</v>
       </c>
       <c r="D30">
         <v>252448.5098952196</v>
@@ -1730,10 +1730,10 @@
         <v>20195.88079161757</v>
       </c>
       <c r="G30">
-        <v>228090.2450734483</v>
+        <v>218779.910672823</v>
       </c>
       <c r="H30">
-        <v>6.064953198237122</v>
+        <v>5.907203881263756</v>
       </c>
       <c r="I30">
         <v>43862.5</v>
@@ -1744,10 +1744,10 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6749.337955599123</v>
+        <v>-3018.573138375094</v>
       </c>
       <c r="C31">
-        <v>2449.816049904835</v>
+        <v>1992.239356555868</v>
       </c>
       <c r="D31">
         <v>257497.480093124</v>
@@ -1759,10 +1759,10 @@
         <v>20599.79840744992</v>
       </c>
       <c r="G31">
-        <v>243647.0196412762</v>
+        <v>233879.108547302</v>
       </c>
       <c r="H31">
-        <v>6.090915546620179</v>
+        <v>5.941337106727618</v>
       </c>
       <c r="I31">
         <v>43862.5</v>

</xml_diff>